<commit_message>
add test for right next bus time
Co-Authored-By: Carl Lagerstedt <105862361+Carl595@users.noreply.github.com>
Co-Authored-By: robinofverberg <91734293+robinofverberg@users.noreply.github.com>
Co-Authored-By: SamuelWidlund <142985254+SamuelWidlund@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/busdata.xlsx
+++ b/data/busdata.xlsx
@@ -1104,9 +1104,9 @@
     </row>
     <row r="14">
       <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="12" t="s">
@@ -1133,9 +1133,10 @@
       <c r="Z14" s="15"/>
     </row>
     <row r="15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="11" t="s">

</xml_diff>